<commit_message>
2024-04-16 Update. Foreseen expirations are now detailed, providing specific days of expiration
</commit_message>
<xml_diff>
--- a/Results/Заклади з таблиці антирабічної допомоги, які мають звітувати в Meddata.xlsx
+++ b/Results/Заклади з таблиці антирабічної допомоги, які мають звітувати в Meddata.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Миколаївська область" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Миколаївська" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -483,6 +483,16 @@
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
+          <t>ПІБ відповідальної особи</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Телефон</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
           <t>Присутній в меддаті?</t>
         </is>
       </c>
@@ -493,7 +503,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Миколаївська область</t>
+          <t>Миколаївська</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -530,6 +540,16 @@
         </is>
       </c>
       <c r="J2" t="inlineStr">
+        <is>
+          <t>Петриченко С.Р.</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>0509501386</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
         <is>
           <t>Ні</t>
         </is>
@@ -541,7 +561,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Миколаївська область</t>
+          <t>Миколаївська</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -578,6 +598,16 @@
         </is>
       </c>
       <c r="J3" t="inlineStr">
+        <is>
+          <t>Дворецька Н.А.</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>06684599911</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
         <is>
           <t>Ні</t>
         </is>
@@ -589,7 +619,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Миколаївська область</t>
+          <t>Миколаївська</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -626,6 +656,16 @@
         </is>
       </c>
       <c r="J4" t="inlineStr">
+        <is>
+          <t>Кожухар О.М.</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>0500702401</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
         <is>
           <t>Ні</t>
         </is>
@@ -637,7 +677,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Миколаївська область</t>
+          <t>Миколаївська</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -674,6 +714,16 @@
         </is>
       </c>
       <c r="J5" t="inlineStr">
+        <is>
+          <t>Домущей Н.А.</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>0634649363</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
         <is>
           <t>Ні</t>
         </is>
@@ -685,7 +735,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Миколаївська область</t>
+          <t>Миколаївська</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -722,6 +772,16 @@
         </is>
       </c>
       <c r="J6" t="inlineStr">
+        <is>
+          <t>Блоховита О.В.</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>0666474378</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
         <is>
           <t>Ні</t>
         </is>
@@ -733,7 +793,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Миколаївська область</t>
+          <t>Миколаївська</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -773,6 +833,16 @@
         </is>
       </c>
       <c r="J7" t="inlineStr">
+        <is>
+          <t>Філіпова Л.Ф.</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>097 562 45 01</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
         <is>
           <t>Ні</t>
         </is>
@@ -784,7 +854,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Миколаївська область</t>
+          <t>Миколаївська</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -821,6 +891,16 @@
         </is>
       </c>
       <c r="J8" t="inlineStr">
+        <is>
+          <t>Мальцева О.М.</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>0508472002</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
         <is>
           <t>Ні</t>
         </is>
@@ -832,7 +912,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Миколаївська область</t>
+          <t>Миколаївська</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -869,6 +949,16 @@
         </is>
       </c>
       <c r="J9" t="inlineStr">
+        <is>
+          <t>Загляда Л.В.</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>0679050435</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
         <is>
           <t>Ні</t>
         </is>
@@ -880,7 +970,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Миколаївська область</t>
+          <t>Миколаївська</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -917,6 +1007,16 @@
         </is>
       </c>
       <c r="J10" t="inlineStr">
+        <is>
+          <t>Калинка Г.В.</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>0988468827</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
         <is>
           <t>Ні</t>
         </is>
@@ -928,7 +1028,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Миколаївська область</t>
+          <t>Миколаївська</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -965,6 +1065,16 @@
         </is>
       </c>
       <c r="J11" t="inlineStr">
+        <is>
+          <t>Омеленчук Г.А.</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>0689975280</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
         <is>
           <t>Ні</t>
         </is>
@@ -976,7 +1086,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Миколаївська область</t>
+          <t>Миколаївська</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -1013,6 +1123,16 @@
         </is>
       </c>
       <c r="J12" t="inlineStr">
+        <is>
+          <t>Петриченко С.Р.</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>0509501386</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
         <is>
           <t>Ні</t>
         </is>
@@ -1024,7 +1144,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Миколаївська область</t>
+          <t>Миколаївська</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -1064,6 +1184,16 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
+          <t>Косенчук О. М.</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>0682379995</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
           <t>Ні</t>
         </is>
       </c>
@@ -1074,7 +1204,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Миколаївська область</t>
+          <t>Миколаївська</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -1111,6 +1241,16 @@
         </is>
       </c>
       <c r="J14" t="inlineStr">
+        <is>
+          <t>Левченко Л.В.</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>0675926126</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
         <is>
           <t>Ні</t>
         </is>
@@ -1122,7 +1262,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Миколаївська область</t>
+          <t>Миколаївська</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -1159,6 +1299,16 @@
         </is>
       </c>
       <c r="J15" t="inlineStr">
+        <is>
+          <t>Слюсаренко О.В.</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>0960773650</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
         <is>
           <t>Ні</t>
         </is>
@@ -1170,7 +1320,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Миколаївська область</t>
+          <t>Миколаївська</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1207,6 +1357,16 @@
         </is>
       </c>
       <c r="J16" t="inlineStr">
+        <is>
+          <t>Черненко О.Б.</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>0962044964</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
         <is>
           <t>Так</t>
         </is>
@@ -1218,7 +1378,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Миколаївська область</t>
+          <t>Миколаївська</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1260,6 +1420,16 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
+          <t>Клиш Л.О.</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>0995019056</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
           <t>Ні</t>
         </is>
       </c>
@@ -1270,7 +1440,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Миколаївська область</t>
+          <t>Миколаївська</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1307,6 +1477,16 @@
         </is>
       </c>
       <c r="J18" t="inlineStr">
+        <is>
+          <t>Волошина Л.О.</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>0677416909</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
         <is>
           <t>Ні</t>
         </is>
@@ -1318,7 +1498,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Миколаївська область</t>
+          <t>Миколаївська</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1366,6 +1546,16 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
+          <t>Стульник І. О</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>0982835217</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
           <t>Ні</t>
         </is>
       </c>
@@ -1376,7 +1566,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Миколаївська область</t>
+          <t>Миколаївська</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1413,6 +1603,16 @@
         </is>
       </c>
       <c r="J20" t="inlineStr">
+        <is>
+          <t>Гаврилюк Д.О.</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>0985828514</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
         <is>
           <t>Ні</t>
         </is>
@@ -1424,7 +1624,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Миколаївська область</t>
+          <t>Миколаївська</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1461,6 +1661,16 @@
         </is>
       </c>
       <c r="J21" t="inlineStr">
+        <is>
+          <t>Лєнчевська Л.В.</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>0957306981</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
         <is>
           <t>Ні</t>
         </is>
@@ -1472,7 +1682,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Миколаївська область</t>
+          <t>Миколаївська</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1509,6 +1719,16 @@
         </is>
       </c>
       <c r="J22" t="inlineStr">
+        <is>
+          <t>Левченко Л.В.</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>0675926126</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
         <is>
           <t>Ні</t>
         </is>
@@ -1520,7 +1740,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Миколаївська область</t>
+          <t>Миколаївська</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1557,6 +1777,16 @@
         </is>
       </c>
       <c r="J23" t="inlineStr">
+        <is>
+          <t>Трушковська Т. С.</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>0982196763</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
         <is>
           <t>Ні</t>
         </is>
@@ -1568,7 +1798,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Миколаївська область</t>
+          <t>Миколаївська</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1605,6 +1835,16 @@
         </is>
       </c>
       <c r="J24" t="inlineStr">
+        <is>
+          <t>Шіллер Л.О.</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>0960242213</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
         <is>
           <t>Ні</t>
         </is>

</xml_diff>